<commit_message>
Agrego modelo de visualizacion de grafo
</commit_message>
<xml_diff>
--- a/backend/core/management/commands/RI_PLAN.xlsx
+++ b/backend/core/management/commands/RI_PLAN.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="337">
   <si>
     <t xml:space="preserve">codigo</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">S31</t>
   </si>
   <si>
-    <t xml:space="preserve">Normal</t>
+    <t xml:space="preserve">carrera</t>
   </si>
   <si>
     <t xml:space="preserve">Inglés III</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">S19</t>
   </si>
   <si>
-    <t xml:space="preserve">Optativa</t>
+    <t xml:space="preserve">electiva</t>
   </si>
   <si>
     <t xml:space="preserve">ESTUDIOS SOCIALES DE LA ECONOMIA (S 19)</t>
@@ -922,15 +922,6 @@
     <t xml:space="preserve">TEORIA POLITICA II (OP 19)</t>
   </si>
   <si>
-    <t xml:space="preserve">GRI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genérica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GENERICA DE RELACIONES INTERNACIONALES (GRI)</t>
-  </si>
-  <si>
     <t xml:space="preserve">GHPRI</t>
   </si>
   <si>
@@ -973,12 +964,12 @@
     <t xml:space="preserve">Política Comparada</t>
   </si>
   <si>
+    <t xml:space="preserve">POLITICA COMPARADA (CP 46)</t>
+  </si>
+  <si>
     <t xml:space="preserve">CC07</t>
   </si>
   <si>
-    <t xml:space="preserve">POLITICA COMPARADA (CP 46)</t>
-  </si>
-  <si>
     <t xml:space="preserve">CP44</t>
   </si>
   <si>
@@ -991,12 +982,12 @@
     <t xml:space="preserve">Historia Latinoamericana</t>
   </si>
   <si>
+    <t xml:space="preserve">Metodología de la Investigación</t>
+  </si>
+  <si>
     <t xml:space="preserve">CC01</t>
   </si>
   <si>
-    <t xml:space="preserve">Metodología de la Investigación</t>
-  </si>
-  <si>
     <t xml:space="preserve">Introducción a la Ciencia Política</t>
   </si>
   <si>
@@ -1004,9 +995,6 @@
   </si>
   <si>
     <t xml:space="preserve">Elementos de Economía</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELEMENTOS DE ECONOMIA (CC06)</t>
   </si>
   <si>
     <t xml:space="preserve">CC05</t>
@@ -1052,7 +1040,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1080,6 +1068,14 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1132,13 +1128,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1333,2704 +1341,2690 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O163"/>
+  <dimension ref="A1:O162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F149" activeCellId="0" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="78.05"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="3" t="n">
         <v>64</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="3" t="n">
         <v>64</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="3" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="K10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="K12" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="K13" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="B14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="K15" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="0" t="s">
+      <c r="B16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="B17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="B18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="0" t="s">
+      <c r="B19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="K20" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K21" s="0" t="s">
+      <c r="K21" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K22" s="0" t="s">
+      <c r="K22" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="I23" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K23" s="0" t="s">
+      <c r="K23" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="I24" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K24" s="0" t="s">
+      <c r="K24" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="I25" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K25" s="0" t="s">
+      <c r="K25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I26" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="K26" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="B27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="B28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="0" t="s">
+      <c r="B29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="0" t="s">
+      <c r="B30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="0" t="s">
+      <c r="B31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="0" t="s">
+      <c r="B32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="0" t="s">
+      <c r="B33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="0" t="s">
+      <c r="B34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="0" t="s">
+      <c r="B35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" s="0" t="s">
+      <c r="B36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" s="0" t="s">
+      <c r="B37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" s="0" t="s">
+      <c r="B38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F39" s="0" t="s">
+      <c r="B39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" s="0" t="s">
+      <c r="B40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="0" t="s">
+      <c r="B41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" s="0" t="s">
+      <c r="B42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F43" s="0" t="s">
+      <c r="B43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" s="0" t="s">
+      <c r="B44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" s="0" t="s">
+      <c r="B45" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F46" s="0" t="s">
+      <c r="B46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F47" s="0" t="s">
+      <c r="B47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F48" s="0" t="s">
+      <c r="B48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B49" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F49" s="0" t="s">
+      <c r="B49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B50" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F50" s="0" t="s">
+      <c r="B50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B51" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F51" s="0" t="s">
+      <c r="B51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F52" s="0" t="s">
+      <c r="B52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F53" s="0" t="s">
+      <c r="B53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B54" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F54" s="0" t="s">
+      <c r="B54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B55" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F55" s="0" t="s">
+      <c r="B55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B56" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F56" s="0" t="s">
+      <c r="B56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B57" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F57" s="0" t="s">
+      <c r="B57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B58" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F58" s="0" t="s">
+      <c r="B58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B59" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F59" s="0" t="s">
+      <c r="B59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B60" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F60" s="0" t="s">
+      <c r="B60" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F61" s="0" t="s">
+      <c r="B61" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B62" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F62" s="0" t="s">
+      <c r="B62" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B63" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F63" s="0" t="s">
+      <c r="B63" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B64" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F64" s="0" t="s">
+      <c r="B64" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B65" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F65" s="0" t="s">
+      <c r="B65" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B66" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F66" s="0" t="s">
+      <c r="B66" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B67" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F67" s="0" t="s">
+      <c r="B67" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B68" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F68" s="0" t="s">
+      <c r="B68" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B69" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F69" s="0" t="s">
+      <c r="B69" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B70" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F70" s="0" t="s">
+      <c r="B70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B71" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F71" s="0" t="s">
+      <c r="B71" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B72" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F72" s="0" t="s">
+      <c r="B72" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B73" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F73" s="0" t="s">
+      <c r="B73" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B74" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F74" s="0" t="s">
+      <c r="B74" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B75" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F75" s="0" t="s">
+      <c r="B75" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B76" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F76" s="0" t="s">
+      <c r="B76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F76" s="3" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F77" s="0" t="s">
+      <c r="B77" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F78" s="0" t="s">
+      <c r="B78" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F79" s="0" t="s">
+      <c r="B79" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F79" s="3" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B80" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F80" s="0" t="s">
+      <c r="B80" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F80" s="3" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B81" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E81" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F81" s="0" t="s">
+      <c r="B81" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F81" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B82" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F82" s="0" t="s">
+      <c r="B82" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B83" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E83" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F83" s="0" t="s">
+      <c r="B83" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B84" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F84" s="0" t="s">
+      <c r="B84" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E85" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F85" s="0" t="s">
+      <c r="B85" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B86" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E86" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F86" s="0" t="s">
+      <c r="B86" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F86" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B87" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F87" s="0" t="s">
+      <c r="B87" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F87" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="A88" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B88" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E88" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F88" s="0" t="s">
+      <c r="B88" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F88" s="3" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B89" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E89" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F89" s="0" t="s">
+      <c r="B89" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F89" s="3" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B90" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E90" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F90" s="0" t="s">
+      <c r="B90" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="A91" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B91" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E91" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F91" s="0" t="s">
+      <c r="B91" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="A92" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B92" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F92" s="0" t="s">
+      <c r="B92" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="A93" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B93" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E93" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F93" s="0" t="s">
+      <c r="B93" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="A94" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B94" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E94" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F94" s="0" t="s">
+      <c r="B94" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B95" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E95" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F95" s="0" t="s">
+      <c r="B95" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F95" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B96" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E96" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F96" s="0" t="s">
+      <c r="B96" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B97" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E97" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F97" s="0" t="s">
+      <c r="B97" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B98" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E98" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F98" s="0" t="s">
+      <c r="B98" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B99" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E99" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F99" s="0" t="s">
+      <c r="B99" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="A100" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B100" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E100" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F100" s="0" t="s">
+      <c r="B100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+      <c r="A101" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B101" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E101" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F101" s="0" t="s">
+      <c r="B101" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="A102" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B102" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E102" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F102" s="0" t="s">
+      <c r="B102" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+      <c r="A103" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B103" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E103" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F103" s="0" t="s">
+      <c r="B103" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F103" s="3" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+      <c r="A104" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B104" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E104" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F104" s="0" t="s">
+      <c r="B104" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F104" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+      <c r="A105" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B105" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E105" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F105" s="0" t="s">
+      <c r="B105" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F105" s="3" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+      <c r="A106" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B106" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E106" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F106" s="0" t="s">
+      <c r="B106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F106" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+      <c r="A107" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B107" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E107" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F107" s="0" t="s">
+      <c r="B107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F107" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+      <c r="A108" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B108" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E108" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F108" s="0" t="s">
+      <c r="B108" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F108" s="3" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="A109" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B109" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E109" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F109" s="0" t="s">
+      <c r="B109" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F109" s="3" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="A110" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B110" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E110" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F110" s="0" t="s">
+      <c r="B110" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F110" s="3" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="A111" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B111" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E111" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F111" s="0" t="s">
+      <c r="B111" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F111" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+      <c r="A112" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B112" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E112" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F112" s="0" t="s">
+      <c r="B112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F112" s="3" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+      <c r="A113" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B113" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E113" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F113" s="0" t="s">
+      <c r="B113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F113" s="3" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+      <c r="A114" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B114" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E114" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F114" s="0" t="s">
+      <c r="B114" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F114" s="3" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+      <c r="A115" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B115" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E115" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F115" s="0" t="s">
+      <c r="B115" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F115" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+      <c r="A116" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B116" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E116" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F116" s="0" t="s">
+      <c r="B116" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F116" s="3" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="A117" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B117" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E117" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F117" s="0" t="s">
+      <c r="B117" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F117" s="3" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+      <c r="A118" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B118" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E118" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F118" s="0" t="s">
+      <c r="B118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F118" s="3" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+      <c r="A119" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B119" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E119" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F119" s="0" t="s">
+      <c r="B119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F119" s="3" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+      <c r="A120" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B120" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E120" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F120" s="0" t="s">
+      <c r="B120" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F120" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="A121" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B121" s="0" t="n">
+      <c r="B121" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D121" s="0" t="n">
+      <c r="D121" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="F121" s="0" t="s">
+      <c r="E121" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F121" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="H121" s="0" t="n">
+      <c r="H121" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I121" s="0" t="n">
+      <c r="I121" s="3" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="A122" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B122" s="0" t="n">
+      <c r="B122" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D122" s="0" t="n">
+      <c r="D122" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="E122" s="0" t="s">
+      <c r="E122" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F122" s="0" t="s">
+      <c r="F122" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="H122" s="0" t="n">
+      <c r="H122" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I122" s="0" t="n">
+      <c r="I122" s="3" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="A123" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B123" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E123" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F123" s="0" t="s">
+      <c r="B123" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F123" s="3" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="A124" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B124" s="0" t="n">
+      <c r="B124" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D124" s="0" t="n">
+      <c r="D124" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E124" s="0" t="s">
+      <c r="E124" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F124" s="0" t="s">
+      <c r="F124" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="H124" s="0" t="n">
+      <c r="H124" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I124" s="0" t="n">
+      <c r="I124" s="3" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+      <c r="A125" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B125" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E125" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F125" s="0" t="s">
+      <c r="B125" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F125" s="3" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+      <c r="A126" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B126" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E126" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F126" s="0" t="s">
+      <c r="B126" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F126" s="3" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
+      <c r="A127" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B127" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E127" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F127" s="0" t="s">
+      <c r="B127" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F127" s="3" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
+      <c r="A128" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B128" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E128" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F128" s="0" t="s">
+      <c r="B128" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F128" s="3" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
+      <c r="A129" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B129" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E129" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F129" s="0" t="s">
+      <c r="B129" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F129" s="3" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+      <c r="A130" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B130" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E130" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F130" s="0" t="s">
+      <c r="B130" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F130" s="3" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
+      <c r="A131" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B131" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E131" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F131" s="0" t="s">
+      <c r="B131" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F131" s="3" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+      <c r="A132" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B132" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E132" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F132" s="0" t="s">
+      <c r="B132" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F132" s="3" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
+      <c r="A133" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B133" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E133" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F133" s="0" t="s">
+      <c r="B133" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F133" s="3" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
+      <c r="A134" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B134" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E134" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F134" s="0" t="s">
+      <c r="B134" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F134" s="3" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
+      <c r="A135" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B135" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E135" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F135" s="0" t="s">
+      <c r="B135" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F135" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
+      <c r="A136" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B136" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E136" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F136" s="0" t="s">
+      <c r="B136" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F136" s="3" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
+      <c r="A137" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B137" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E137" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F137" s="0" t="s">
+      <c r="B137" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F137" s="3" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
+      <c r="A138" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B138" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E138" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F138" s="0" t="s">
+      <c r="B138" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F138" s="3" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+      <c r="A139" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B139" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E139" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F139" s="0" t="s">
+      <c r="B139" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F139" s="3" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+      <c r="A140" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B140" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E140" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F140" s="0" t="s">
+      <c r="B140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F140" s="3" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
+      <c r="A141" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B141" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E141" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F141" s="0" t="s">
+      <c r="B141" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F141" s="3" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
+      <c r="A142" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B142" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E142" s="0" t="s">
+      <c r="B142" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D142" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F142" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="F142" s="0" t="s">
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="3" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
+      <c r="B143" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F143" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B143" s="0" t="n">
+      <c r="I143" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B144" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B145" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B146" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D146" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D143" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E143" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="F143" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="I143" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="B144" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E144" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F144" s="0" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="B145" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E145" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F145" s="0" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+      <c r="E146" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F146" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="B146" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E146" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F146" s="0" t="s">
+    </row>
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="3" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+      <c r="B147" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F147" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="B147" s="0" t="n">
+      <c r="H147" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I147" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="K147" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B148" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D147" s="0" t="n">
+      <c r="D148" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="E147" s="0" t="s">
+      <c r="E148" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F147" s="0" t="s">
+      <c r="F148" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="H147" s="0" t="n">
+      <c r="B149" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="H149" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I147" s="0" t="n">
+      <c r="I149" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K147" s="0" t="s">
+      <c r="K149" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B150" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D150" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B151" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D151" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H151" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I151" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="K151" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="B148" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E148" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F148" s="0" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
+      <c r="B152" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D152" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="H152" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I152" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="K152" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="B149" s="0" t="n">
+      <c r="B153" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D153" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="H153" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I153" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="K153" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B154" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D154" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="H154" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I154" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B155" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D155" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="D149" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E149" s="0" t="s">
+      <c r="E155" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F149" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="H149" s="0" t="n">
+      <c r="F155" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="H155" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I155" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="K155" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B156" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D156" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B157" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D157" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H157" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I157" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="K157" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B158" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H158" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I158" s="3" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B159" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D159" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H159" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I159" s="3" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B160" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B161" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="H161" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I149" s="0" t="n">
+      <c r="I161" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K149" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="B150" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E150" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F150" s="0" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="B151" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D151" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E151" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F151" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="H151" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I151" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="K151" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="B152" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D152" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E152" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F152" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="H152" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I152" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="K152" s="0" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B153" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D153" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E153" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F153" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="H153" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I153" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="K153" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="B154" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D154" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E154" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F154" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="H154" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I154" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="K154" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="B155" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D155" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E155" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="F155" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="H155" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I155" s="0" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="B156" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E156" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F156" s="0" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="B157" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D157" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E157" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F157" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="H157" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I157" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="K157" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B158" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D158" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E158" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F158" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="H158" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I158" s="0" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="B159" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D159" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E159" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F159" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="H159" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I159" s="0" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="B160" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E160" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F160" s="0" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="B161" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D161" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E161" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F161" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="H161" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I161" s="0" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="B162" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E162" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F162" s="0" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="B163" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E163" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F163" s="0" t="s">
-        <v>340</v>
-      </c>
-    </row>
+    </row>
+    <row r="162" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Agrego filtro por materias aprobadas
</commit_message>
<xml_diff>
--- a/backend/core/management/commands/RI_PLAN.xlsx
+++ b/backend/core/management/commands/RI_PLAN.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="337">
   <si>
     <t xml:space="preserve">codigo</t>
   </si>
@@ -982,10 +982,10 @@
     <t xml:space="preserve">Historia Latinoamericana</t>
   </si>
   <si>
+    <t xml:space="preserve">CC01</t>
+  </si>
+  <si>
     <t xml:space="preserve">Metodología de la Investigación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC01</t>
   </si>
   <si>
     <t xml:space="preserve">Introducción a la Ciencia Política</t>
@@ -1040,7 +1040,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1068,14 +1068,6 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1128,7 +1120,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1142,10 +1134,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1343,8 +1331,8 @@
   </sheetPr>
   <dimension ref="A1:O162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F149" activeCellId="0" sqref="F149"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A135" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K151" activeCellId="0" sqref="K151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3690,6 +3678,9 @@
       <c r="F146" s="3" t="s">
         <v>309</v>
       </c>
+      <c r="K146" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
@@ -3797,7 +3788,7 @@
         <v>64</v>
       </c>
       <c r="K151" s="3" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,7 +3805,7 @@
         <v>16</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H152" s="3" t="n">
         <v>6</v>
@@ -3823,7 +3814,7 @@
         <v>96</v>
       </c>
       <c r="K152" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3900,7 +3891,7 @@
       <c r="I155" s="3" t="n">
         <v>64</v>
       </c>
-      <c r="K155" s="4" t="s">
+      <c r="K155" s="3" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3969,7 +3960,7 @@
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B159" s="3" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Agrego detalle breve de carrera
</commit_message>
<xml_diff>
--- a/backend/core/management/commands/RI_PLAN.xlsx
+++ b/backend/core/management/commands/RI_PLAN.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$O$161</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="340">
   <si>
     <t xml:space="preserve">codigo</t>
   </si>
@@ -70,6 +73,9 @@
     <t xml:space="preserve">S31</t>
   </si>
   <si>
+    <t xml:space="preserve">Avanzado</t>
+  </si>
+  <si>
     <t xml:space="preserve">carrera</t>
   </si>
   <si>
@@ -82,10 +88,16 @@
     <t xml:space="preserve">S30</t>
   </si>
   <si>
+    <t xml:space="preserve">General</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inglés II</t>
   </si>
   <si>
     <t xml:space="preserve">S29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Básico</t>
   </si>
   <si>
     <t xml:space="preserve">Inglés I</t>
@@ -1146,7 +1158,28 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1326,13 +1359,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A135" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K151" activeCellId="0" sqref="K151"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C155" activeCellId="0" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1395,14 +1428,17 @@
       <c r="B2" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D2" s="3" t="n">
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>4</v>
@@ -1411,24 +1447,27 @@
         <v>64</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D3" s="3" t="n">
         <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>4</v>
@@ -1437,24 +1476,27 @@
         <v>64</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D4" s="3" t="n">
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>4</v>
@@ -1463,35 +1505,38 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D6" s="3" t="n">
         <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>6</v>
@@ -1500,24 +1545,27 @@
         <v>96</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D7" s="3" t="n">
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>6</v>
@@ -1526,24 +1574,27 @@
         <v>96</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D8" s="3" t="n">
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>6</v>
@@ -1552,24 +1603,27 @@
         <v>96</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D9" s="3" t="n">
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>6</v>
@@ -1578,24 +1632,27 @@
         <v>96</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D10" s="3" t="n">
         <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>6</v>
@@ -1604,24 +1661,27 @@
         <v>96</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D11" s="3" t="n">
         <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>6</v>
@@ -1630,24 +1690,27 @@
         <v>96</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D12" s="3" t="n">
         <v>5</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>6</v>
@@ -1656,24 +1719,27 @@
         <v>96</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D13" s="3" t="n">
         <v>6</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>6</v>
@@ -1682,38 +1748,41 @@
         <v>96</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D15" s="3" t="n">
         <v>4</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H15" s="3" t="n">
         <v>6</v>
@@ -1722,80 +1791,83 @@
         <v>96</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B18" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B19" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B20" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D20" s="3" t="n">
         <v>9</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H20" s="3" t="n">
         <v>6</v>
@@ -1804,24 +1876,27 @@
         <v>96</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B21" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D21" s="3" t="n">
         <v>8</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H21" s="3" t="n">
         <v>6</v>
@@ -1830,24 +1905,27 @@
         <v>96</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B22" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D22" s="3" t="n">
         <v>7</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H22" s="3" t="n">
         <v>6</v>
@@ -1856,24 +1934,27 @@
         <v>96</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B23" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D23" s="3" t="n">
         <v>8</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H23" s="3" t="n">
         <v>6</v>
@@ -1882,24 +1963,27 @@
         <v>96</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B24" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D24" s="3" t="n">
         <v>7</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H24" s="3" t="n">
         <v>6</v>
@@ -1908,24 +1992,27 @@
         <v>96</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B25" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C25" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D25" s="3" t="n">
         <v>7</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H25" s="3" t="n">
         <v>6</v>
@@ -1934,24 +2021,27 @@
         <v>96</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B26" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D26" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H26" s="3" t="n">
         <v>6</v>
@@ -1960,1340 +2050,1343 @@
         <v>96</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B27" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B28" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B29" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B30" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B31" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B32" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B33" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B34" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B35" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B36" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B37" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B38" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B39" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B40" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B41" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B42" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B43" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B44" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B45" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B46" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B47" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B48" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B49" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B50" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B51" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B52" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B53" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B54" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B55" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B56" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B57" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B58" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B59" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B60" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B61" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B62" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B63" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B64" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B65" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B66" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B67" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B68" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B69" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B70" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B71" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B72" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B73" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B74" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B75" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B76" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B77" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B78" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B79" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B80" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B81" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B82" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B83" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B84" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B85" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B86" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B87" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B88" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B89" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B90" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B91" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B92" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B93" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B94" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B95" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B96" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B97" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B98" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B99" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B100" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B101" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B102" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B103" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B104" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B105" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B106" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B107" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B108" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B109" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B110" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B111" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B112" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B113" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B114" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B115" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B116" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B117" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B118" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B119" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B120" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B121" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C121" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D121" s="3" t="n">
         <v>9</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="H121" s="3" t="n">
         <v>4</v>
@@ -3304,19 +3397,22 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B122" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C122" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D122" s="3" t="n">
         <v>9</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="H122" s="3" t="n">
         <v>4</v>
@@ -3325,35 +3421,38 @@
         <v>64</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B123" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B124" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="C124" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D124" s="3" t="n">
         <v>8</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="H124" s="3" t="n">
         <v>4</v>
@@ -3362,338 +3461,344 @@
         <v>64</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B125" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B126" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B127" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B128" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B129" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B130" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B131" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B132" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B133" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B134" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B135" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B136" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B137" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B138" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B139" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B140" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B141" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B142" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C142" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D142" s="3" t="n">
         <v>9</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B143" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="I143" s="3" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B144" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B145" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B146" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="C146" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D146" s="3" t="n">
         <v>5</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="K146" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B147" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="H147" s="3" t="n">
         <v>6</v>
@@ -3702,38 +3807,44 @@
         <v>96</v>
       </c>
       <c r="K147" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B148" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="C148" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D148" s="3" t="n">
         <v>5</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B149" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="C149" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="E149" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="H149" s="3" t="n">
         <v>6</v>
@@ -3742,44 +3853,50 @@
         <v>96</v>
       </c>
       <c r="K149" s="3" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B150" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C150" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D150" s="3" t="n">
         <v>4</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="K150" s="3" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B151" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C151" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D151" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="H151" s="3" t="n">
         <v>6</v>
@@ -3788,24 +3905,27 @@
         <v>64</v>
       </c>
       <c r="K151" s="3" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B152" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C152" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D152" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="H152" s="3" t="n">
         <v>6</v>
@@ -3814,24 +3934,27 @@
         <v>96</v>
       </c>
       <c r="K152" s="3" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B153" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="C153" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D153" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="H153" s="3" t="n">
         <v>6</v>
@@ -3840,24 +3963,27 @@
         <v>96</v>
       </c>
       <c r="K153" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B154" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="C154" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D154" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="H154" s="3" t="n">
         <v>4</v>
@@ -3866,24 +3992,27 @@
         <v>64</v>
       </c>
       <c r="K154" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B155" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="C155" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D155" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="H155" s="3" t="n">
         <v>4</v>
@@ -3892,41 +4021,47 @@
         <v>64</v>
       </c>
       <c r="K155" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B156" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="C156" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D156" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B157" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="C157" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D157" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="H157" s="3" t="n">
         <v>4</v>
@@ -3935,21 +4070,21 @@
         <v>64</v>
       </c>
       <c r="K157" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B158" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="H158" s="3" t="n">
         <v>4</v>
@@ -3960,19 +4095,22 @@
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B159" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="C159" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D159" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="H159" s="3" t="n">
         <v>4</v>
@@ -3981,32 +4119,32 @@
         <v>64</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B160" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B161" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="H161" s="3" t="n">
         <v>6</v>
@@ -4017,6 +4155,13 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A1:O161">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="carrera"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4024,5 +4169,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agrego aproximacion a calendario academico
</commit_message>
<xml_diff>
--- a/backend/core/management/commands/RI_PLAN.xlsx
+++ b/backend/core/management/commands/RI_PLAN.xlsx
@@ -1359,13 +1359,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O162"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C155" activeCellId="0" sqref="C155"/>
+      <selection pane="topLeft" activeCell="J159" activeCellId="0" sqref="J159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1446,6 +1446,9 @@
       <c r="I2" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="J2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K2" s="3" t="s">
         <v>19</v>
       </c>
@@ -1475,6 +1478,9 @@
       <c r="I3" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1504,8 +1510,11 @@
       <c r="I4" s="3" t="n">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1544,6 +1553,9 @@
       <c r="I6" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1573,6 +1585,9 @@
       <c r="I7" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J7" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K7" s="3" t="s">
         <v>34</v>
       </c>
@@ -1602,6 +1617,9 @@
       <c r="I8" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K8" s="3" t="s">
         <v>37</v>
       </c>
@@ -1631,6 +1649,9 @@
       <c r="I9" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K9" s="3" t="s">
         <v>40</v>
       </c>
@@ -1660,6 +1681,9 @@
       <c r="I10" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1689,6 +1713,9 @@
       <c r="I11" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J11" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K11" s="3" t="s">
         <v>44</v>
       </c>
@@ -1718,6 +1745,9 @@
       <c r="I12" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K12" s="3" t="s">
         <v>44</v>
       </c>
@@ -1747,11 +1777,14 @@
       <c r="I13" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J13" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K13" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>48</v>
       </c>
@@ -1790,11 +1823,14 @@
       <c r="I15" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K15" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>51</v>
       </c>
@@ -1808,7 +1844,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
@@ -1822,7 +1858,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>55</v>
       </c>
@@ -1836,7 +1872,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -1875,6 +1911,9 @@
       <c r="I20" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J20" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K20" s="3" t="s">
         <v>61</v>
       </c>
@@ -1904,6 +1943,9 @@
       <c r="I21" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J21" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K21" s="3" t="s">
         <v>64</v>
       </c>
@@ -1933,6 +1975,9 @@
       <c r="I22" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J22" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1962,6 +2007,9 @@
       <c r="I23" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J23" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1991,6 +2039,9 @@
       <c r="I24" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J24" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K24" s="3" t="s">
         <v>70</v>
       </c>
@@ -2020,6 +2071,9 @@
       <c r="I25" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J25" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K25" s="3" t="s">
         <v>40</v>
       </c>
@@ -2049,11 +2103,14 @@
       <c r="I26" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J26" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K26" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>75</v>
       </c>
@@ -2067,7 +2124,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
@@ -2081,7 +2138,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>79</v>
       </c>
@@ -2095,7 +2152,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>81</v>
       </c>
@@ -2109,7 +2166,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>83</v>
       </c>
@@ -2123,7 +2180,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>85</v>
       </c>
@@ -2137,7 +2194,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>87</v>
       </c>
@@ -2151,7 +2208,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>89</v>
       </c>
@@ -2165,7 +2222,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
@@ -2179,7 +2236,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>93</v>
       </c>
@@ -2193,7 +2250,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
@@ -2207,7 +2264,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>97</v>
       </c>
@@ -2221,7 +2278,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>99</v>
       </c>
@@ -2235,7 +2292,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>101</v>
       </c>
@@ -2249,7 +2306,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>103</v>
       </c>
@@ -2263,7 +2320,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>105</v>
       </c>
@@ -2277,7 +2334,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>107</v>
       </c>
@@ -2291,7 +2348,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
         <v>109</v>
       </c>
@@ -2305,7 +2362,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>111</v>
       </c>
@@ -2319,7 +2376,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>113</v>
       </c>
@@ -2333,7 +2390,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
         <v>115</v>
       </c>
@@ -2347,7 +2404,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
         <v>117</v>
       </c>
@@ -2361,7 +2418,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
         <v>119</v>
       </c>
@@ -2375,7 +2432,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
         <v>121</v>
       </c>
@@ -2389,7 +2446,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
         <v>123</v>
       </c>
@@ -2403,7 +2460,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
         <v>125</v>
       </c>
@@ -2417,7 +2474,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
         <v>127</v>
       </c>
@@ -2431,7 +2488,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
         <v>129</v>
       </c>
@@ -2445,7 +2502,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>131</v>
       </c>
@@ -2459,7 +2516,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
         <v>133</v>
       </c>
@@ -2473,7 +2530,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>135</v>
       </c>
@@ -2487,7 +2544,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
         <v>137</v>
       </c>
@@ -2501,7 +2558,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
         <v>139</v>
       </c>
@@ -2515,7 +2572,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
         <v>141</v>
       </c>
@@ -2529,7 +2586,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
         <v>143</v>
       </c>
@@ -2543,7 +2600,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
         <v>145</v>
       </c>
@@ -2557,7 +2614,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
         <v>147</v>
       </c>
@@ -2571,7 +2628,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
         <v>149</v>
       </c>
@@ -2585,7 +2642,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
         <v>151</v>
       </c>
@@ -2599,7 +2656,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
         <v>153</v>
       </c>
@@ -2613,7 +2670,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
         <v>155</v>
       </c>
@@ -2627,7 +2684,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
         <v>157</v>
       </c>
@@ -2641,7 +2698,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
         <v>159</v>
       </c>
@@ -2655,7 +2712,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
         <v>161</v>
       </c>
@@ -2669,7 +2726,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
         <v>163</v>
       </c>
@@ -2683,7 +2740,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
         <v>165</v>
       </c>
@@ -2697,7 +2754,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
         <v>167</v>
       </c>
@@ -2711,7 +2768,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
         <v>169</v>
       </c>
@@ -2725,7 +2782,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
         <v>171</v>
       </c>
@@ -2739,7 +2796,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
         <v>173</v>
       </c>
@@ -2753,7 +2810,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
         <v>175</v>
       </c>
@@ -2767,7 +2824,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
         <v>177</v>
       </c>
@@ -2781,7 +2838,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
         <v>179</v>
       </c>
@@ -2795,7 +2852,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
         <v>181</v>
       </c>
@@ -2809,7 +2866,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
         <v>183</v>
       </c>
@@ -2823,7 +2880,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
         <v>185</v>
       </c>
@@ -2837,7 +2894,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
         <v>187</v>
       </c>
@@ -2851,7 +2908,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
         <v>189</v>
       </c>
@@ -2865,7 +2922,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
         <v>191</v>
       </c>
@@ -2879,7 +2936,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
         <v>193</v>
       </c>
@@ -2893,7 +2950,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
         <v>195</v>
       </c>
@@ -2907,7 +2964,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
         <v>197</v>
       </c>
@@ -2921,7 +2978,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
         <v>199</v>
       </c>
@@ -2935,7 +2992,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
         <v>201</v>
       </c>
@@ -2949,7 +3006,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
         <v>203</v>
       </c>
@@ -2963,7 +3020,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
         <v>205</v>
       </c>
@@ -2977,7 +3034,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
         <v>207</v>
       </c>
@@ -2991,7 +3048,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
         <v>209</v>
       </c>
@@ -3005,7 +3062,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
         <v>211</v>
       </c>
@@ -3019,7 +3076,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
         <v>213</v>
       </c>
@@ -3033,7 +3090,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
         <v>215</v>
       </c>
@@ -3047,7 +3104,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
         <v>217</v>
       </c>
@@ -3061,7 +3118,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
         <v>219</v>
       </c>
@@ -3075,7 +3132,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
         <v>221</v>
       </c>
@@ -3089,7 +3146,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
         <v>223</v>
       </c>
@@ -3103,7 +3160,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
         <v>225</v>
       </c>
@@ -3117,7 +3174,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
         <v>227</v>
       </c>
@@ -3131,7 +3188,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
         <v>229</v>
       </c>
@@ -3145,7 +3202,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
         <v>231</v>
       </c>
@@ -3159,7 +3216,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
         <v>233</v>
       </c>
@@ -3173,7 +3230,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
         <v>235</v>
       </c>
@@ -3187,7 +3244,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
         <v>237</v>
       </c>
@@ -3201,7 +3258,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
         <v>239</v>
       </c>
@@ -3215,7 +3272,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
         <v>241</v>
       </c>
@@ -3229,7 +3286,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
         <v>243</v>
       </c>
@@ -3243,7 +3300,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
         <v>245</v>
       </c>
@@ -3257,7 +3314,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
         <v>247</v>
       </c>
@@ -3271,7 +3328,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
         <v>249</v>
       </c>
@@ -3285,7 +3342,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
         <v>251</v>
       </c>
@@ -3299,7 +3356,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
         <v>253</v>
       </c>
@@ -3313,7 +3370,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
         <v>255</v>
       </c>
@@ -3327,7 +3384,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
         <v>257</v>
       </c>
@@ -3341,7 +3398,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
         <v>259</v>
       </c>
@@ -3355,7 +3412,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
         <v>261</v>
       </c>
@@ -3394,6 +3451,9 @@
       <c r="I121" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="J121" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
@@ -3420,8 +3480,11 @@
       <c r="I122" s="3" t="n">
         <v>64</v>
       </c>
-    </row>
-    <row r="123" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J122" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
         <v>19</v>
       </c>
@@ -3460,8 +3523,11 @@
       <c r="I124" s="3" t="n">
         <v>64</v>
       </c>
-    </row>
-    <row r="125" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J124" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
         <v>268</v>
       </c>
@@ -3475,7 +3541,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
         <v>271</v>
       </c>
@@ -3489,7 +3555,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
         <v>273</v>
       </c>
@@ -3503,7 +3569,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
         <v>275</v>
       </c>
@@ -3517,7 +3583,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
         <v>277</v>
       </c>
@@ -3531,7 +3597,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
         <v>279</v>
       </c>
@@ -3545,7 +3611,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
         <v>281</v>
       </c>
@@ -3559,7 +3625,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
         <v>283</v>
       </c>
@@ -3573,7 +3639,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
         <v>285</v>
       </c>
@@ -3587,7 +3653,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
         <v>287</v>
       </c>
@@ -3601,7 +3667,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
         <v>289</v>
       </c>
@@ -3615,7 +3681,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
         <v>291</v>
       </c>
@@ -3629,7 +3695,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
         <v>293</v>
       </c>
@@ -3643,7 +3709,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
         <v>295</v>
       </c>
@@ -3657,7 +3723,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
         <v>297</v>
       </c>
@@ -3671,7 +3737,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
         <v>299</v>
       </c>
@@ -3685,7 +3751,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
         <v>301</v>
       </c>
@@ -3718,8 +3784,11 @@
       <c r="F142" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="143" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J142" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
         <v>305</v>
       </c>
@@ -3736,7 +3805,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
         <v>307</v>
       </c>
@@ -3750,7 +3819,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
         <v>309</v>
       </c>
@@ -3783,11 +3852,14 @@
       <c r="F146" s="3" t="s">
         <v>312</v>
       </c>
+      <c r="J146" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K146" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
         <v>313</v>
       </c>
@@ -3829,6 +3901,9 @@
       <c r="F148" s="3" t="s">
         <v>316</v>
       </c>
+      <c r="J148" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
@@ -3852,6 +3927,9 @@
       <c r="I149" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J149" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K149" s="3" t="s">
         <v>318</v>
       </c>
@@ -3875,6 +3953,9 @@
       <c r="F150" s="3" t="s">
         <v>320</v>
       </c>
+      <c r="J150" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K150" s="3" t="s">
         <v>318</v>
       </c>
@@ -3904,6 +3985,9 @@
       <c r="I151" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="J151" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K151" s="3" t="s">
         <v>323</v>
       </c>
@@ -3933,6 +4017,9 @@
       <c r="I152" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J152" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K152" s="3" t="s">
         <v>323</v>
       </c>
@@ -3962,6 +4049,9 @@
       <c r="I153" s="3" t="n">
         <v>96</v>
       </c>
+      <c r="J153" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K153" s="3" t="s">
         <v>74</v>
       </c>
@@ -3991,6 +4081,9 @@
       <c r="I154" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="J154" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K154" s="3" t="s">
         <v>74</v>
       </c>
@@ -4020,6 +4113,9 @@
       <c r="I155" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="J155" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K155" s="3" t="s">
         <v>74</v>
       </c>
@@ -4043,6 +4139,9 @@
       <c r="F156" s="3" t="s">
         <v>330</v>
       </c>
+      <c r="J156" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
@@ -4069,11 +4168,14 @@
       <c r="I157" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="J157" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K157" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="s">
         <v>333</v>
       </c>
@@ -4118,8 +4220,11 @@
       <c r="I159" s="3" t="n">
         <v>64</v>
       </c>
-    </row>
-    <row r="160" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J159" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
         <v>336</v>
       </c>
@@ -4133,7 +4238,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="s">
         <v>338</v>
       </c>
@@ -4155,13 +4260,7 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:O161">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="carrera"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O161"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>